<commit_message>
update uart and gitnore
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCMUT\HK242\Mirco_Controller\Project\Traffic_Light\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3ADAB30-DC61-4511-93C4-9B039F2B257B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E84971E-D7A6-4777-B744-AE754C9E0598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9420" xr2:uid="{2530A35B-1B37-4992-86C9-41023F7DE64E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Kit pic mini ra chân 16F877/16F887/18F4550</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>Hàng Rào Đực Đơn 2.54mm 40 Chân 1 Hàng Cao 11.2mm Xuyên Lỗ Mạ Vàng, 1x40 chân, Mạ vàng</t>
+  </si>
+  <si>
+    <t>LCD I2C 16x2</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>USB UART CP2102</t>
   </si>
 </sst>
 </file>
@@ -498,7 +507,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,20 +665,38 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="2">
-        <f>SUM(D1:D8)</f>
-        <v>530900</v>
-      </c>
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>

</xml_diff>